<commit_message>
Make file paths dynamic & Update README.md
</commit_message>
<xml_diff>
--- a/testData/InstantVideoConsultation.xlsx
+++ b/testData/InstantVideoConsultation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="13">
   <si>
     <t>Gynaecology</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Urology</t>
+  </si>
+  <si>
+    <t>₹599</t>
+  </si>
+  <si>
+    <t>₹549</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -465,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -473,7 +479,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -481,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -489,7 +495,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -497,7 +503,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -505,7 +511,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -513,7 +519,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>